<commit_message>
Bug fixing and SOAP Read Write
</commit_message>
<xml_diff>
--- a/TestCase Remittance.xlsx
+++ b/TestCase Remittance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Test Case</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>TC01</t>
-  </si>
-  <si>
-    <t>N_GenerateOTP</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>Login</t>
@@ -88,12 +82,15 @@
 </t>
   </si>
   <si>
+    <t>/services/partners</t>
+  </si>
+  <si>
     <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
 &lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/" xmlns:ns1="https://api.shmart.in"&gt;
     &lt;SOAP-ENV:Body&gt;
         &lt;ns1:LoginResponse&gt;
             &lt;return&gt;
-                &lt;SessionID&gt;298C36B901&lt;/SessionID&gt;
+                &lt;SessionID&gt;B6B1AA1A99&lt;/SessionID&gt;
                 &lt;ResponseCode&gt;0&lt;/ResponseCode&gt;
                 &lt;ResponseMessage&gt;Successful&lt;/ResponseMessage&gt;
             &lt;/return&gt;
@@ -102,7 +99,80 @@
 &lt;/SOAP-ENV:Envelope&gt;</t>
   </si>
   <si>
-    <t>/services/partners</t>
+    <t>SessionID</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/" xmlns:ns1="https://api.shmart.in"&gt;
+    &lt;SOAP-ENV:Body&gt;
+        &lt;ns1:LoginResponse&gt;
+            &lt;return&gt;
+                &lt;ResponseMessage&gt;Invalid Login&lt;/ResponseMessage&gt;
+                &lt;ResponseCode&gt;100&lt;/ResponseCode&gt;
+            &lt;/return&gt;
+        &lt;/ns1:LoginResponse&gt;
+    &lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>P_Valid  Login</t>
+  </si>
+  <si>
+    <t>N_invalid_Login</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/"
+xmlns:sas="http://api.shmart.in/"&gt;
+&lt;SOAP-ENV:Body&gt;
+        &lt;sas:Login&gt;
+                &lt;Username&gt;#random_string&lt;/Username&gt;
+                &lt;Password&gt;pratik&lt;/Password&gt;
+        &lt;/sas:Login&gt;
+&lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/"
+xmlns:sas="http://api.shmart.in/"&gt;
+&lt;SOAP-ENV:Body&gt;
+        &lt;sas:GenerateOTPRequest&gt;
+                &lt;SessionID&gt;DC421FA156&lt;/SessionID&gt;
+                &lt;ProductCode&gt;27&lt;/ProductCode&gt;
+                &lt;Mobile&gt;9833868977&lt;/Mobile&gt;
+                &lt;RequestType&gt;R&lt;/RequestType&gt;
+         &lt;/sas:GenerateOTPRequest&gt;
+&lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/" xmlns:ns1="https://api.shmart.in"&gt;
+    &lt;SOAP-ENV:Body&gt;
+        &lt;ns1:GenerateOTPRequestResponse&gt;
+            &lt;return&gt;
+                &lt;ResponseMessage&gt;Invalid Login&lt;/ResponseMessage&gt;
+                &lt;ResponseCode&gt;100&lt;/ResponseCode&gt;
+            &lt;/return&gt;
+        &lt;/ns1:GenerateOTPRequestResponse&gt;
+    &lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>N_invalid_Session</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>Parameters to write</t>
   </si>
 </sst>
 </file>
@@ -163,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -175,6 +245,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -504,11 +577,11 @@
     <col min="5" max="5" width="7.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="20" style="4" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="40" style="4" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="4" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,42 +613,103 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="168.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="I2" s="2">
         <v>400</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="146.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="157.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifying 500 and uat environment changes
</commit_message>
<xml_diff>
--- a/TestCase Remittance.xlsx
+++ b/TestCase Remittance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Test Case</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>TC01</t>
-  </si>
-  <si>
-    <t>N_GenerateOTP</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>Login</t>
@@ -88,12 +82,15 @@
 </t>
   </si>
   <si>
+    <t>/services/partners</t>
+  </si>
+  <si>
     <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
 &lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/" xmlns:ns1="https://api.shmart.in"&gt;
     &lt;SOAP-ENV:Body&gt;
         &lt;ns1:LoginResponse&gt;
             &lt;return&gt;
-                &lt;SessionID&gt;298C36B901&lt;/SessionID&gt;
+                &lt;SessionID&gt;B6B1AA1A99&lt;/SessionID&gt;
                 &lt;ResponseCode&gt;0&lt;/ResponseCode&gt;
                 &lt;ResponseMessage&gt;Successful&lt;/ResponseMessage&gt;
             &lt;/return&gt;
@@ -102,7 +99,80 @@
 &lt;/SOAP-ENV:Envelope&gt;</t>
   </si>
   <si>
-    <t>/services/partners</t>
+    <t>SessionID</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/" xmlns:ns1="https://api.shmart.in"&gt;
+    &lt;SOAP-ENV:Body&gt;
+        &lt;ns1:LoginResponse&gt;
+            &lt;return&gt;
+                &lt;ResponseMessage&gt;Invalid Login&lt;/ResponseMessage&gt;
+                &lt;ResponseCode&gt;100&lt;/ResponseCode&gt;
+            &lt;/return&gt;
+        &lt;/ns1:LoginResponse&gt;
+    &lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>P_Valid  Login</t>
+  </si>
+  <si>
+    <t>N_invalid_Login</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/"
+xmlns:sas="http://api.shmart.in/"&gt;
+&lt;SOAP-ENV:Body&gt;
+        &lt;sas:Login&gt;
+                &lt;Username&gt;#random_string&lt;/Username&gt;
+                &lt;Password&gt;pratik&lt;/Password&gt;
+        &lt;/sas:Login&gt;
+&lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/"
+xmlns:sas="http://api.shmart.in/"&gt;
+&lt;SOAP-ENV:Body&gt;
+        &lt;sas:GenerateOTPRequest&gt;
+                &lt;SessionID&gt;DC421FA156&lt;/SessionID&gt;
+                &lt;ProductCode&gt;27&lt;/ProductCode&gt;
+                &lt;Mobile&gt;9833868977&lt;/Mobile&gt;
+                &lt;RequestType&gt;R&lt;/RequestType&gt;
+         &lt;/sas:GenerateOTPRequest&gt;
+&lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;SOAP-ENV:Envelope xmlns:SOAP-ENV="http://schemas.xmlsoap.org/soap/envelope/" xmlns:ns1="https://api.shmart.in"&gt;
+    &lt;SOAP-ENV:Body&gt;
+        &lt;ns1:GenerateOTPRequestResponse&gt;
+            &lt;return&gt;
+                &lt;ResponseMessage&gt;Invalid Login&lt;/ResponseMessage&gt;
+                &lt;ResponseCode&gt;100&lt;/ResponseCode&gt;
+            &lt;/return&gt;
+        &lt;/ns1:GenerateOTPRequestResponse&gt;
+    &lt;/SOAP-ENV:Body&gt;
+&lt;/SOAP-ENV:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>N_invalid_Session</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>Parameters to write</t>
   </si>
 </sst>
 </file>
@@ -163,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -175,6 +245,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -504,11 +577,11 @@
     <col min="5" max="5" width="7.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="20" style="4" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="40" style="4" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="4" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,42 +613,103 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="168.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="I2" s="2">
         <v>400</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="146.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="157.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>